<commit_message>
Delete unused interfaces, create global services
</commit_message>
<xml_diff>
--- a/Lection 3/task 3.1/ReportApp/Reports/ActivityReport.xlsx
+++ b/Lection 3/task 3.1/ReportApp/Reports/ActivityReport.xlsx
@@ -27,7 +27,7 @@
     <x:t xml:space="preserve">Generated by: </x:t>
   </x:si>
   <x:si>
-    <x:t>Soul Of Cinder (Admin)</x:t>
+    <x:t>John Snow (Client)</x:t>
   </x:si>
   <x:si>
     <x:t>Report</x:t>
@@ -36,9 +36,6 @@
     <x:t>Client</x:t>
   </x:si>
   <x:si>
-    <x:t>Admin</x:t>
-  </x:si>
-  <x:si>
     <x:t>First name</x:t>
   </x:si>
   <x:si>
@@ -54,15 +51,6 @@
     <x:t>Additional Info</x:t>
   </x:si>
   <x:si>
-    <x:t>Name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pronouns</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Works At</x:t>
-  </x:si>
-  <x:si>
     <x:t>John</x:t>
   </x:si>
   <x:si>
@@ -76,15 +64,6 @@
   </x:si>
   <x:si>
     <x:t>Killed the Queen on working hours</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Final boss</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Soul/Soul</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Klin of the First Flame</x:t>
   </x:si>
   <x:si>
     <x:t>Didn't piss of the Wall</x:t>
@@ -577,7 +556,7 @@
   <x:dimension ref="A2:I11"/>
   <x:sheetViews>
     <x:sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <x:selection activeCell="I9" sqref="I9"/>
+      <x:selection activeCell="I9" sqref="I9 G9:F9"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,9 +567,7 @@
     <x:col min="4" max="4" width="10.424911" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="13.710625" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="31.853482" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="9.710625" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="9.853482" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="23.996339" style="0" customWidth="1"/>
+    <x:col min="7" max="9" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -621,9 +598,6 @@
       <x:c r="D7" s="7"/>
       <x:c r="E7" s="7"/>
       <x:c r="F7" s="7"/>
-      <x:c r="G7" s="7"/>
-      <x:c r="H7" s="7"/>
-      <x:c r="I7" s="7"/>
     </x:row>
     <x:row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="B8" s="8" t="s">
@@ -633,303 +607,130 @@
       <x:c r="D8" s="8"/>
       <x:c r="E8" s="8"/>
       <x:c r="F8" s="8"/>
-      <x:c r="G8" s="8" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="H8" s="8"/>
-      <x:c r="I8" s="8"/>
     </x:row>
     <x:row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B9" s="9" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C9" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C9" s="9" t="s">
+      <x:c r="D9" s="9" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="D9" s="9" t="s">
+      <x:c r="E9" s="9" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="E9" s="9" t="s">
+      <x:c r="F9" s="9" t="s">
         <x:v>10</x:v>
-      </x:c>
-      <x:c r="F9" s="9" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="G9" s="9" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="H9" s="9" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="I9" s="9" t="s">
-        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="B10" s="10" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C10" s="10" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D10" s="10" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E10" s="10" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F10" s="10" t="s">
         <x:v>15</x:v>
-      </x:c>
-      <x:c r="C10" s="10" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D10" s="10" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E10" s="10" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F10" s="10" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G10" s="10" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H10" s="10" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I10" s="10" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="B11" s="11" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C11" s="11" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D11" s="11" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E11" s="11" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F11" s="11" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="D11" s="11" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E11" s="11" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F11" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G11" s="11" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H11" s="11" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I11" s="11" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:9">
       <x:c r="B12" s="10" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C12" s="10" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D12" s="10" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E12" s="10" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F12" s="10" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="D12" s="10" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E12" s="10" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F12" s="10" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G12" s="10" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H12" s="10" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I12" s="10" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:9">
       <x:c r="B13" s="11" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C13" s="11" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D13" s="11" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E13" s="11" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F13" s="11" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="D13" s="11" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E13" s="11" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F13" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G13" s="11" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H13" s="11" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I13" s="11" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:9">
       <x:c r="B14" s="10" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C14" s="10" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D14" s="10" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E14" s="10" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F14" s="10" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="D14" s="10" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E14" s="10" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F14" s="10" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G14" s="10" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H14" s="10" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I14" s="10" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:9">
       <x:c r="B15" s="11" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C15" s="11" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D15" s="11" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E15" s="11" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F15" s="11" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="D15" s="11" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E15" s="11" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F15" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G15" s="11" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H15" s="11" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I15" s="11" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:9">
-      <x:c r="B16" s="10" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C16" s="10" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D16" s="10" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E16" s="10" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F16" s="10" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G16" s="10" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H16" s="10" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I16" s="10" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:9">
-      <x:c r="B17" s="11" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C17" s="11" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D17" s="11" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E17" s="11" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F17" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G17" s="11" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H17" s="11" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I17" s="11" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:9">
-      <x:c r="B18" s="10" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C18" s="10" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D18" s="10" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E18" s="10" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F18" s="10" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G18" s="10" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H18" s="10" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I18" s="10" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:9">
-      <x:c r="B19" s="11" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C19" s="11" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D19" s="11" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E19" s="11" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F19" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G19" s="11" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H19" s="11" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I19" s="11" t="s">
-        <x:v>22</x:v>
-      </x:c>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="3">
-    <x:mergeCell ref="B7:I7"/>
+  <x:mergeCells count="2">
+    <x:mergeCell ref="B7:F7"/>
     <x:mergeCell ref="B8:F8"/>
-    <x:mergeCell ref="G8:I8"/>
   </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Handled all issue about task (49 and more)
</commit_message>
<xml_diff>
--- a/Lection 3/task 3.1/ReportApp/Reports/ActivityReport.xlsx
+++ b/Lection 3/task 3.1/ReportApp/Reports/ActivityReport.xlsx
@@ -27,7 +27,7 @@
     <x:t xml:space="preserve">Generated by: </x:t>
   </x:si>
   <x:si>
-    <x:t>John Snow (Client)</x:t>
+    <x:t>Soul Of Cinder (Admin)</x:t>
   </x:si>
   <x:si>
     <x:t>Report</x:t>
@@ -36,6 +36,9 @@
     <x:t>Client</x:t>
   </x:si>
   <x:si>
+    <x:t>Admin</x:t>
+  </x:si>
+  <x:si>
     <x:t>First name</x:t>
   </x:si>
   <x:si>
@@ -51,6 +54,15 @@
     <x:t>Additional Info</x:t>
   </x:si>
   <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pronouns</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Works At</x:t>
+  </x:si>
+  <x:si>
     <x:t>John</x:t>
   </x:si>
   <x:si>
@@ -64,6 +76,15 @@
   </x:si>
   <x:si>
     <x:t>Killed the Queen on working hours</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Final boss</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Soul/Soul</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Klin of the First Flame</x:t>
   </x:si>
   <x:si>
     <x:t>Didn't piss of the Wall</x:t>
@@ -556,7 +577,7 @@
   <x:dimension ref="A2:I11"/>
   <x:sheetViews>
     <x:sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <x:selection activeCell="I9" sqref="I9 G9:F9"/>
+      <x:selection activeCell="I9" sqref="I9"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +588,9 @@
     <x:col min="4" max="4" width="10.424911" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="13.710625" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="31.853482" style="0" customWidth="1"/>
-    <x:col min="7" max="9" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="9.710625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="9.853482" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="23.996339" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -598,6 +621,9 @@
       <x:c r="D7" s="7"/>
       <x:c r="E7" s="7"/>
       <x:c r="F7" s="7"/>
+      <x:c r="G7" s="7"/>
+      <x:c r="H7" s="7"/>
+      <x:c r="I7" s="7"/>
     </x:row>
     <x:row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="B8" s="8" t="s">
@@ -607,130 +633,303 @@
       <x:c r="D8" s="8"/>
       <x:c r="E8" s="8"/>
       <x:c r="F8" s="8"/>
+      <x:c r="G8" s="8" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H8" s="8"/>
+      <x:c r="I8" s="8"/>
     </x:row>
     <x:row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B9" s="9" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C9" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D9" s="9" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E9" s="9" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F9" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="G9" s="9" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H9" s="9" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="I9" s="9" t="s">
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="B10" s="10" t="s">
-        <x:v>11</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C10" s="10" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D10" s="10" t="s">
-        <x:v>13</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E10" s="10" t="s">
-        <x:v>14</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F10" s="10" t="s">
-        <x:v>15</x:v>
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G10" s="10" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H10" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I10" s="10" t="s">
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="B11" s="11" t="s">
-        <x:v>11</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C11" s="11" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D11" s="11" t="s">
-        <x:v>13</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E11" s="11" t="s">
-        <x:v>14</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F11" s="11" t="s">
-        <x:v>16</x:v>
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G11" s="11" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H11" s="11" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I11" s="11" t="s">
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:9">
       <x:c r="B12" s="10" t="s">
-        <x:v>11</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C12" s="10" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D12" s="10" t="s">
-        <x:v>13</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E12" s="10" t="s">
-        <x:v>14</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F12" s="10" t="s">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G12" s="10" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H12" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I12" s="10" t="s">
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:9">
       <x:c r="B13" s="11" t="s">
-        <x:v>11</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C13" s="11" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D13" s="11" t="s">
-        <x:v>13</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E13" s="11" t="s">
-        <x:v>14</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F13" s="11" t="s">
-        <x:v>16</x:v>
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G13" s="11" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H13" s="11" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I13" s="11" t="s">
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:9">
       <x:c r="B14" s="10" t="s">
-        <x:v>11</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C14" s="10" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D14" s="10" t="s">
-        <x:v>13</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E14" s="10" t="s">
-        <x:v>14</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F14" s="10" t="s">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G14" s="10" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H14" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I14" s="10" t="s">
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:9">
       <x:c r="B15" s="11" t="s">
-        <x:v>11</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C15" s="11" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="D15" s="11" t="s">
-        <x:v>13</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E15" s="11" t="s">
-        <x:v>14</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="F15" s="11" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G15" s="11" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H15" s="11" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I15" s="11" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:9">
+      <x:c r="B16" s="10" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C16" s="10" t="s">
         <x:v>16</x:v>
       </x:c>
+      <x:c r="D16" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E16" s="10" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F16" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G16" s="10" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H16" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I16" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:9">
+      <x:c r="B17" s="11" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C17" s="11" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D17" s="11" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E17" s="11" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F17" s="11" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G17" s="11" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H17" s="11" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I17" s="11" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:9">
+      <x:c r="B18" s="10" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C18" s="10" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D18" s="10" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E18" s="10" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F18" s="10" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G18" s="10" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H18" s="10" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I18" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:9">
+      <x:c r="B19" s="11" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C19" s="11" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D19" s="11" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E19" s="11" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F19" s="11" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G19" s="11" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H19" s="11" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I19" s="11" t="s">
+        <x:v>22</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="2">
-    <x:mergeCell ref="B7:F7"/>
+  <x:mergeCells count="3">
+    <x:mergeCell ref="B7:I7"/>
     <x:mergeCell ref="B8:F8"/>
+    <x:mergeCell ref="G8:I8"/>
   </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Simplified RequestsService and ReportConfigurationService
</commit_message>
<xml_diff>
--- a/Lection 3/task 3.1/ReportApp/Reports/ActivityReport.xlsx
+++ b/Lection 3/task 3.1/ReportApp/Reports/ActivityReport.xlsx
@@ -27,7 +27,7 @@
     <x:t xml:space="preserve">Generated by: </x:t>
   </x:si>
   <x:si>
-    <x:t>Soul Of Cinder (Admin)</x:t>
+    <x:t>John Snow (Client)</x:t>
   </x:si>
   <x:si>
     <x:t>Report</x:t>
@@ -36,9 +36,6 @@
     <x:t>Client</x:t>
   </x:si>
   <x:si>
-    <x:t>Admin</x:t>
-  </x:si>
-  <x:si>
     <x:t>First name</x:t>
   </x:si>
   <x:si>
@@ -54,15 +51,6 @@
     <x:t>Additional Info</x:t>
   </x:si>
   <x:si>
-    <x:t>Name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pronouns</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Works At</x:t>
-  </x:si>
-  <x:si>
     <x:t>John</x:t>
   </x:si>
   <x:si>
@@ -76,15 +64,6 @@
   </x:si>
   <x:si>
     <x:t>Killed the Queen on working hours</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Final boss</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Soul/Soul</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Klin of the First Flame</x:t>
   </x:si>
   <x:si>
     <x:t>Didn't piss of the Wall</x:t>
@@ -577,7 +556,7 @@
   <x:dimension ref="A2:I11"/>
   <x:sheetViews>
     <x:sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <x:selection activeCell="I9" sqref="I9"/>
+      <x:selection activeCell="I9" sqref="I9 G9:F9"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,9 +567,7 @@
     <x:col min="4" max="4" width="10.424911" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="13.710625" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="31.853482" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="9.710625" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="9.853482" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="23.996339" style="0" customWidth="1"/>
+    <x:col min="7" max="9" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -621,9 +598,6 @@
       <x:c r="D7" s="7"/>
       <x:c r="E7" s="7"/>
       <x:c r="F7" s="7"/>
-      <x:c r="G7" s="7"/>
-      <x:c r="H7" s="7"/>
-      <x:c r="I7" s="7"/>
     </x:row>
     <x:row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="B8" s="8" t="s">
@@ -633,303 +607,130 @@
       <x:c r="D8" s="8"/>
       <x:c r="E8" s="8"/>
       <x:c r="F8" s="8"/>
-      <x:c r="G8" s="8" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="H8" s="8"/>
-      <x:c r="I8" s="8"/>
     </x:row>
     <x:row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="B9" s="9" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C9" s="9" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C9" s="9" t="s">
+      <x:c r="D9" s="9" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="D9" s="9" t="s">
+      <x:c r="E9" s="9" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="E9" s="9" t="s">
+      <x:c r="F9" s="9" t="s">
         <x:v>10</x:v>
-      </x:c>
-      <x:c r="F9" s="9" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="G9" s="9" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="H9" s="9" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="I9" s="9" t="s">
-        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="B10" s="10" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C10" s="10" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D10" s="10" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E10" s="10" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F10" s="10" t="s">
         <x:v>15</x:v>
-      </x:c>
-      <x:c r="C10" s="10" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D10" s="10" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E10" s="10" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F10" s="10" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G10" s="10" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H10" s="10" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I10" s="10" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="B11" s="11" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C11" s="11" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D11" s="11" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E11" s="11" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F11" s="11" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="D11" s="11" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E11" s="11" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F11" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G11" s="11" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H11" s="11" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I11" s="11" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:9">
       <x:c r="B12" s="10" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C12" s="10" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D12" s="10" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E12" s="10" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F12" s="10" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="D12" s="10" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E12" s="10" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F12" s="10" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G12" s="10" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H12" s="10" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I12" s="10" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:9">
       <x:c r="B13" s="11" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C13" s="11" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D13" s="11" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E13" s="11" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F13" s="11" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="D13" s="11" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E13" s="11" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F13" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G13" s="11" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H13" s="11" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I13" s="11" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:9">
       <x:c r="B14" s="10" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C14" s="10" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D14" s="10" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E14" s="10" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F14" s="10" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="D14" s="10" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E14" s="10" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F14" s="10" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G14" s="10" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H14" s="10" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I14" s="10" t="s">
-        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:9">
       <x:c r="B15" s="11" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C15" s="11" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D15" s="11" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E15" s="11" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F15" s="11" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="D15" s="11" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E15" s="11" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F15" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G15" s="11" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H15" s="11" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I15" s="11" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:9">
-      <x:c r="B16" s="10" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C16" s="10" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D16" s="10" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E16" s="10" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F16" s="10" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G16" s="10" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H16" s="10" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I16" s="10" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:9">
-      <x:c r="B17" s="11" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C17" s="11" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D17" s="11" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E17" s="11" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F17" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G17" s="11" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H17" s="11" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I17" s="11" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:9">
-      <x:c r="B18" s="10" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C18" s="10" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D18" s="10" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E18" s="10" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F18" s="10" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G18" s="10" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H18" s="10" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I18" s="10" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:9">
-      <x:c r="B19" s="11" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C19" s="11" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D19" s="11" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E19" s="11" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F19" s="11" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G19" s="11" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H19" s="11" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I19" s="11" t="s">
-        <x:v>22</x:v>
-      </x:c>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="3">
-    <x:mergeCell ref="B7:I7"/>
+  <x:mergeCells count="2">
+    <x:mergeCell ref="B7:F7"/>
     <x:mergeCell ref="B8:F8"/>
-    <x:mergeCell ref="G8:I8"/>
   </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>